<commit_message>
format and title case
</commit_message>
<xml_diff>
--- a/templates/TransactionReport.xlsx
+++ b/templates/TransactionReport.xlsx
@@ -75,6 +75,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -142,6 +146,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +440,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,9 +455,9 @@
     <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -480,13 +492,13 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">

</xml_diff>